<commit_message>
se agregaron las carpetas con los archivos respectivos del cuarto trimestre y se actualizaron unos documentos
</commit_message>
<xml_diff>
--- a/02_Levantamiento de informacion/Encuesta clientes (respuestas).xlsx
+++ b/02_Levantamiento de informacion/Encuesta clientes (respuestas).xlsx
@@ -534,12 +534,10 @@
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -784,9 +782,9 @@
       <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="23" width="18.88"/>
+    <col customWidth="1" min="1" max="23" width="21.57"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>